<commit_message>
Add Supplier(Subcontracted to) and Instrument on Methods Import Change typo _Method to Method and add Instrument  - defaultmethod and defaultinstrument on AS Import
</commit_message>
<xml_diff>
--- a/src/bika/lims/setupdata/test/test.xlsx
+++ b/src/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="58"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3800" uniqueCount="1510">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -4715,10 +4715,10 @@
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
-    <numFmt numFmtId="168" formatCode="DD\-MM\-YYYY;@"/>
-    <numFmt numFmtId="169" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
+    <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="170" formatCode="#"/>
   </numFmts>
   <fonts count="31">
@@ -5773,7 +5773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5783,10 +5783,9 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5843,7 +5842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5853,12 +5852,11 @@
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="19.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6180,7 +6178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6190,7 +6188,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.32421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.54"/>
@@ -6203,7 +6201,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.32"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6368,7 +6365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6378,13 +6375,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="12.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6547,7 +6543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6557,15 +6553,14 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6773,7 +6768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6783,11 +6778,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6883,7 +6877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6893,18 +6887,15 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="0" width="6.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="5.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="5.79"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="13.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7320,7 +7311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7330,17 +7321,16 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="9" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="5.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="5.68"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7616,7 +7606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7626,13 +7616,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="4" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="5.14"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7689,7 +7678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7699,14 +7688,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="56.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="81" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7950,7 +7938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7960,11 +7948,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8091,7 +8078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8101,12 +8088,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.41"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8489,7 +8475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8499,13 +8485,11 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="6" style="0" width="9.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.8"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8720,7 +8704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8730,11 +8714,10 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="2" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8999,7 +8982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9009,11 +8992,10 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9119,39 +9101,37 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U16" activeCellId="0" sqref="U16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="21.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="21" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="26.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10299,7 +10279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -10309,7 +10289,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.75"/>
@@ -10323,7 +10303,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="38.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="20.7" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10490,7 +10469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -10500,7 +10479,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.78"/>
@@ -10513,7 +10492,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10673,7 +10651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -10683,15 +10661,14 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.02"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10811,7 +10788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -10821,19 +10798,18 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11680,7 +11656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -11690,11 +11666,11 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.03"/>
@@ -11702,7 +11678,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="14.9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11907,7 +11882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -11917,7 +11892,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.09"/>
@@ -11928,7 +11903,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="14.9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12009,7 +11983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -12019,22 +11993,19 @@
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="30.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13083,7 +13054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13093,12 +13064,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="21.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13186,7 +13156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13196,12 +13166,11 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.32421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="6.32"/>
   </cols>
   <sheetData>
     <row r="1" s="129" customFormat="true" ht="14.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13324,7 +13293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13334,12 +13303,11 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13980,17 +13948,17 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X4" activeCellId="0" sqref="X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.56"/>
@@ -14001,7 +13969,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="81" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="81" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="81" width="10.6"/>
@@ -14012,12 +13979,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="3.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="24.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14294,7 +14260,9 @@
         <v>1</v>
       </c>
       <c r="W4" s="141"/>
-      <c r="X4" s="145"/>
+      <c r="X4" s="145" t="s">
+        <v>639</v>
+      </c>
       <c r="Y4" s="145"/>
       <c r="Z4" s="143" t="n">
         <v>10</v>
@@ -16270,10 +16238,6 @@
       <formula1>Methods!$A$4:$A$84</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select an instrument from the selection list. Maintain the list of valid options on the 'Instruments' sheet" promptTitle="Select a valid Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X4" type="list">
-      <formula1>Instruments!$A$1:$A$24</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Calculation from the selection list. Maintain the list of valid options on the 'Calculations' sheet" promptTitle="Select a valid Calculation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y4:Y28" type="list">
       <formula1>Calculations!$A$4:$A$97</formula1>
       <formula2>0</formula2>
@@ -16298,6 +16262,10 @@
       <formula1>'Analysis Service Uncertainties'!$A$4:$A$43</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select an instrument from the selection list. Maintain the list of valid options on the 'Instruments' sheet" promptTitle="Select a valid Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X4" type="list">
+      <formula1>Instruments!$B$1:$B$24</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -16310,7 +16278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16320,11 +16288,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="61" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16361,7 +16328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16371,11 +16338,10 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16412,7 +16378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16422,14 +16388,13 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16484,7 +16449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16494,14 +16459,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="973" min="5" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="974" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="974" style="0" width="5.14"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="24.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16693,7 +16656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16703,13 +16666,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="5" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="998" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="998" style="0" width="5.14"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="24.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18170,7 +18132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -18180,15 +18142,14 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18324,7 +18285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -18334,13 +18295,12 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18517,7 +18477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -18527,12 +18487,11 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="29.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="29.66"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18758,7 +18717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -18768,7 +18727,7 @@
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.74"/>
@@ -18776,7 +18735,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15.05" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24250,7 +24208,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24260,7 +24218,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.92"/>
@@ -24269,7 +24227,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24413,7 +24370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24423,12 +24380,11 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24591,7 +24547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24601,14 +24557,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24660,7 +24615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24670,13 +24625,12 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24826,7 +24780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24836,13 +24790,11 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25265,7 +25217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25275,9 +25227,9 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.64453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.03"/>
@@ -25287,11 +25239,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="9.64"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25412,7 +25363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25422,14 +25373,13 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.64453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.64"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25522,7 +25472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25532,12 +25482,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.64453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.49"/>
@@ -25547,7 +25497,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="96.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="9.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25674,7 +25623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25684,15 +25633,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="8.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="36" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25836,7 +25784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25846,14 +25794,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="19.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25914,7 +25861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25924,10 +25871,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.8"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="22.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -25980,7 +25924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25990,11 +25934,10 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26063,7 +26006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26073,7 +26016,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.64453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
@@ -26083,9 +26026,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="9.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26194,7 +26135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26204,11 +26145,11 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.64453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.49"/>
@@ -26217,7 +26158,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="9.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26414,7 +26354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26424,14 +26364,13 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="26.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26492,7 +26431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26502,12 +26441,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26570,7 +26508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26580,11 +26518,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26650,7 +26587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26660,14 +26597,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27047,25 +26983,24 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="5.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="23.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27466,7 +27401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -27476,14 +27411,14 @@
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.07"/>
@@ -27497,10 +27432,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="7.71"/>
   </cols>
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27923,7 +27856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -27933,7 +27866,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
@@ -27942,7 +27875,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" s="73" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29193,7 +29125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -29203,7 +29135,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.95"/>
@@ -29214,11 +29146,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="15" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="15" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="27" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29822,7 +29753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -29832,11 +29763,10 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="19.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29889,7 +29819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -29899,11 +29829,10 @@
       <selection pane="topLeft" activeCell="O60" activeCellId="0" sqref="O60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>